<commit_message>
Case wide, 2025, instance 1 klar for show
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\V8\Master_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE35D3F4-1EA4-478C-984C-EF3E9D8BC619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0979459-F55C-4249-AC3F-B916FF048AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -81,36 +81,18 @@
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{FB04843D-B295-40BA-A00D-5E6B2A5753A5}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
-        </r>
       </text>
     </comment>
     <comment ref="B7" authorId="1" shapeId="0" xr:uid="{5B616586-A621-4A9A-8B8B-B24C9A3AFD46}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -125,19 +107,10 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{C5776892-1F20-4F03-80A7-219BD90F0AD8}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -152,19 +125,10 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{FA6AF892-F62D-433D-A1F3-B906131A1ADB}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -179,19 +143,10 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{4AB2F2FD-D9AF-4EF6-975B-D27067AE3E61}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -206,19 +161,10 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{38A2CE00-8A9F-411D-8730-D3AF28BB4DFB}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -1315,7 +1261,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -3041,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>656.04987334112695</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,7 +3037,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>10.68421476851921</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3099,7 +3045,7 @@
         <v>73</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>15.414421127453631</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,7 +3077,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>312.3093481178044</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3952,7 +3898,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,7 +3956,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>9.4023667116569634</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>50.249746921488892</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +3993,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,7 +4051,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>9.4023667116569634</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4113,7 +4059,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>3032.3123142277782</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6692,6 +6638,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6892,41 +6858,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6949,9 +6884,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
max case deep, 2025
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0979459-F55C-4249-AC3F-B916FF048AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC0DC9D-0B87-4B04-89F4-C56970F633BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +2988,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>656.04987334112695</v>
+        <v>571.21638006553064</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>10.68421476851921</v>
+        <v>30.336889218799971</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3045,7 +3045,7 @@
         <v>73</v>
       </c>
       <c r="B7">
-        <v>15.414421127453631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>312.3093481178044</v>
+        <v>192.50876985941579</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,7 +3956,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>9.4023667116569634</v>
+        <v>20.161143399817799</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>50.249746921488892</v>
+        <v>72.733635921664771</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4051,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>9.4023667116569634</v>
+        <v>20.161143399817799</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>3032.3123142277782</v>
+        <v>4389.0987194108056</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,15 +6638,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6655,6 +6646,15 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6859,14 +6859,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6879,6 +6871,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
max case wide 2050
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC0DC9D-0B87-4B04-89F4-C56970F633BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566BF894-1514-4F19-9FDF-E6C0907FC2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +2988,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>571.21638006553064</v>
+        <v>657.37493915294976</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>30.336889218799971</v>
+        <v>33.674558060421809</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6.8403724883951904</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>7.6841550260775211</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>192.50876985941579</v>
+        <v>256.06471528657181</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>67</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>37.65235806637677</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,7 +3932,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>20.430082072832331</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>20.161143399817799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>72.733635921664771</v>
+        <v>55.075160928370025</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,7 +4027,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>20.430082072832331</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>20.161143399817799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4389.0987194108056</v>
+        <v>3323.5010905050881</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,6 +6638,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6646,15 +6655,6 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6859,6 +6859,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6871,14 +6879,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
2050 max case deep
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566BF894-1514-4F19-9FDF-E6C0907FC2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDE22D3-9F95-420E-98AE-4FE1F0817279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -2987,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>657.37493915294976</v>
+        <v>620.79602332002491</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>33.674558060421809</v>
+        <v>36.278382817546991</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>6.8403724883951904</v>
+        <v>20.921766955491421</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>7.6841550260775211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>256.06471528657181</v>
+        <v>182.63963689447331</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>67</v>
       </c>
       <c r="B17">
-        <v>37.65235806637677</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3897,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,7 +3932,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>20.430082072832331</v>
+        <v>31.85432685547071</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>55.075160928370025</v>
+        <v>72.824918601155787</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="B4" sqref="B4:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,7 +4027,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>20.430082072832331</v>
+        <v>31.85432685547071</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>3323.5010905050881</v>
+        <v>4394.6071569662981</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,15 +6638,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6655,6 +6646,15 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6859,14 +6859,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6879,6 +6871,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
2025 deep klar for trøkk
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDE22D3-9F95-420E-98AE-4FE1F0817279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54191CBC-6387-4E32-88AD-523EA8A19552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -1261,7 +1261,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>620.79602332002491</v>
+        <v>571.21640000000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>36.278382817546991</v>
+        <v>30.336889218799971</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>20.921766955491421</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>182.63963689447331</v>
+        <v>192.50876985941579</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3932,7 +3932,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>31.85432685547071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>20.161143399817799</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>72.824918601155787</v>
+        <v>72.733635921664771</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,7 +4027,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>31.85432685547071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>20.161143399817799</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4394.6071569662981</v>
+        <v>4389.0987194108056</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,6 +6638,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6646,15 +6655,6 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6859,6 +6859,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6871,14 +6879,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Dummy 2025 klar for max
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojviken\OneDrive\Dokumenter\10. semester\Til master\Kjøre kode\14.05\Max_case_pulp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Max_case_Pulp\Max_case_P-P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54191CBC-6387-4E32-88AD-523EA8A19552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F7629D-52C5-42F7-82F0-5EA7D9819624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -81,18 +81,36 @@
   <commentList>
     <comment ref="B6" authorId="0" shapeId="0" xr:uid="{FB04843D-B295-40BA-A00D-5E6B2A5753A5}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
     <comment ref="B7" authorId="1" shapeId="0" xr:uid="{5B616586-A621-4A9A-8B8B-B24C9A3AFD46}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -107,10 +125,19 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{C5776892-1F20-4F03-80A7-219BD90F0AD8}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -125,10 +152,19 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{FA6AF892-F62D-433D-A1F3-B906131A1ADB}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -143,10 +179,19 @@
   <commentList>
     <comment ref="C37" authorId="0" shapeId="0" xr:uid="{4AB2F2FD-D9AF-4EF6-975B-D27067AE3E61}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT sell</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -161,10 +206,19 @@
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{38A2CE00-8A9F-411D-8730-D3AF28BB4DFB}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     RT buy</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -2987,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,7 +3083,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>571.21640000000002</v>
+        <v>1114.9839999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +3091,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>30.336889218799971</v>
+        <v>39.165999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3077,7 +3131,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>192.50876985941579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,7 +3952,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,7 +4010,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>20.161143399817799</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +4018,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>72.733635921664771</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3992,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4105,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>20.161143399817799</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4059,7 +4113,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4389.0987194108056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6638,15 +6692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
@@ -6655,6 +6700,15 @@
     <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6859,14 +6913,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -6879,6 +6925,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Klar for kjøring med investering
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Max_case_Pulp\Max_case_P-P\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE49D12-FA6F-4607-9194-35A4A34CE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C4D9EF-8188-429C-ABCD-2778088F5AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="795" windowWidth="27915" windowHeight="14535" tabRatio="1000" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="795" windowWidth="27915" windowHeight="14535" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -3041,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3083,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>558.20040817281097</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,7 +3091,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>34.9911934283245</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>83.850282349994004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>61</v>
       </c>
       <c r="B11">
-        <v>249.95017381391901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3952,7 +3952,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,7 +3986,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>36.772006618627501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,8 +4018,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <f>2.9/175*(4281.82812378375)</f>
-        <v>70.956008908416422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,7 +4081,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>36.772006618627501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4114,7 +4113,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>4281.82812378375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6693,26 +6692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6913,32 +6892,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6955,4 +6929,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Klar for dummy uten storage
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Max_case_Pulp\Max_case_P-P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Out_of_sample_dummy\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C4D9EF-8188-429C-ABCD-2778088F5AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC91B28-C1A7-4AB0-90F1-53FEFFEE9F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="795" windowWidth="27915" windowHeight="14535" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="765" windowWidth="27915" windowHeight="14535" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -3042,7 +3042,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3083,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,7 +3091,7 @@
         <v>72</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>73</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,6 +6692,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6892,27 +6912,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6929,29 +6954,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Klar for dummy med storage
</commit_message>
<xml_diff>
--- a/Input_data_With_dummyGrid_and_RT.xlsx
+++ b/Input_data_With_dummyGrid_and_RT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Simple_extended\Out_of_sample_dummy\Max_case_pulp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC91B28-C1A7-4AB0-90F1-53FEFFEE9F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCB9AF-F3C6-4245-BB23-9B3ECFDD89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="765" windowWidth="27915" windowHeight="14535" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_AvailableExcessHeat" sheetId="8" r:id="rId1"/>
@@ -3952,7 +3952,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,7 +4010,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,7 +4105,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6692,26 +6692,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -6912,32 +6892,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6954,4 +6929,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>